<commit_message>
Stabilized generate_response logic and passed full test suite (55/55)
</commit_message>
<xml_diff>
--- a/docs/unit_test_cases.xlsx
+++ b/docs/unit_test_cases.xlsx
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
@@ -615,7 +615,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update exported Selenium and unit test case reports
</commit_message>
<xml_diff>
--- a/docs/unit_test_cases.xlsx
+++ b/docs/unit_test_cases.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,166 +486,406 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>test_bias_logic.py</t>
+          <t>test_ingredients_scenarios.py</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>test_bias_cultural_sensitivity</t>
+          <t>test_additional_ingredient_scenarios</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>test_response_logic.py</t>
+          <t>test_ingredients_scenarios.py</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>test_known_ingredients</t>
+          <t>test_chicken_and_rice</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>test_response_logic.py</t>
+          <t>test_ingredients_scenarios.py</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>test_equipment_detection</t>
+          <t>test_chicken_lemon_parsley</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>test_response_logic.py</t>
+          <t>test_ingredients_scenarios.py</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>test_restricted_ingredient_response</t>
+          <t>test_empty_ingredient_list</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>test_response_logic.py</t>
+          <t>test_ingredients_scenarios.py</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>test_unsure_user_input</t>
+          <t>test_conflicting_restrictions</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>test_response_logic.py</t>
+          <t>test_ingredients_scenarios.py</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>test_empty_input</t>
+          <t>test_gibberish_input</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>21</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>test_response_logic.py</t>
+          <t>test_bias_logic.py</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>test_bias_trigger</t>
+          <t>test_bias_cultural_sensitivity</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>test_response_logic.py</t>
+          <t>test_allergy_scenarios.py</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>test_safe_prompt</t>
+          <t>test_common_restriction_prompts</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>test_response_logic.py</t>
+          <t>test_allergy_scenarios.py</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>test_gendered_prompt</t>
+          <t>test_peanut_allergy</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>test_response_logic.py</t>
+          <t>test_allergy_scenarios.py</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>test_cultural_stereotype</t>
+          <t>test_gluten_free</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>test_allergy_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>test_dairy_free</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>test_allergy_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>test_religious_restriction</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>test_allergy_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>test_multi_axis_prompts</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>test_allergy_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>test_ambiguous_cases</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>test_equipment_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>test_common_equipment_prompts</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>test_equipment_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>test_instant_pot_chicken_rice</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>test_equipment_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>test_slow_cooker_soup</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>test_equipment_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>test_oven_bake_conflict</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>test_equipment_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>test_air_fryer_dessert</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>test_equipment_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>test_wok_stirfry</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>test_equipment_scenarios.py</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>test_microwave_restriction</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>test_response_logic.py</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>test_bias_cultural_sensitivity</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>41</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>test_known_ingredients</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>test_response_logic.py</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>test_equipment_detection</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>test_response_logic.py</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>test_restricted_ingredient_response</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>test_response_logic.py</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>test_unsure_user_input</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>test_response_logic.py</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>test_empty_input</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>test_response_logic.py</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>test_bias_trigger</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>